<commit_message>
New input data files for testing.
New input data files for testing.
</commit_message>
<xml_diff>
--- a/input_data/input_data_2.xlsx
+++ b/input_data/input_data_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vttgroup-my.sharepoint.com/personal/dennis_sundell_vtt_fi1/Documents/Documents/HOPE/Predicer/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{A6342B90-F8EE-4C3F-8710-409C3F73327A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C211487-688B-4840-BCEC-AA2FA013DB33}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="13_ncr:1_{A6342B90-F8EE-4C3F-8710-409C3F73327A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD22C75B-BAD3-4388-AB1F-4C4CD305F426}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="16" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>node</t>
   </si>
@@ -113,9 +113,6 @@
     <t>ramp_up</t>
   </si>
   <si>
-    <t>spot</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -209,40 +206,22 @@
     <t>operator</t>
   </si>
   <si>
-    <t>ng, ALL</t>
-  </si>
-  <si>
     <t>residual_value</t>
   </si>
   <si>
     <t>elc1</t>
   </si>
   <si>
-    <t>npe1</t>
-  </si>
-  <si>
-    <t>npe2</t>
-  </si>
-  <si>
-    <t>elc2</t>
-  </si>
-  <si>
     <t>gt1</t>
   </si>
   <si>
-    <t>gt2</t>
-  </si>
-  <si>
     <t>spot1</t>
   </si>
   <si>
-    <t>spot2</t>
-  </si>
-  <si>
-    <t>npe1,s1</t>
-  </si>
-  <si>
-    <t>npe2,s1</t>
+    <t>npe,s1</t>
+  </si>
+  <si>
+    <t>ng, s1</t>
   </si>
 </sst>
 </file>
@@ -626,7 +605,7 @@
   <dimension ref="A1:A49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A32"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +615,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -650,9 +629,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>44671.08333321759</v>
-      </c>
+      <c r="A4" s="7"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -799,7 +776,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C30"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,10 +786,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -834,12 +811,9 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -993,72 +967,56 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
@@ -1081,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DDD9A-EF34-4108-8532-230729E9C708}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D32"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,18 +1052,15 @@
     <col min="6" max="13" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -1113,11 +1068,8 @@
       <c r="B2">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -1125,89 +1077,80 @@
       <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
@@ -1278,7 +1221,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,15 +1231,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -1304,10 +1247,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1320,22 +1263,22 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1361,7 +1304,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1379,9 +1322,9 @@
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
+        <v/>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -1535,7 +1478,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1551,9 +1494,9 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -1692,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5704FC51-737E-45F9-9A9E-85A96AFE5439}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1705,10 +1648,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1740,7 +1683,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1756,9 +1699,9 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -1907,7 +1850,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1923,9 +1866,9 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -2061,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1B16B-CDA9-46BD-BA51-731AA9327652}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2091,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>6</v>
@@ -2109,13 +2052,13 @@
         <v>5</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2158,13 +2101,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="6">
         <v>0</v>
       </c>
       <c r="C3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -2176,13 +2119,13 @@
         <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J3" s="6">
         <v>0</v>
@@ -2196,31 +2139,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6">
         <v>0</v>
       </c>
       <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
       <c r="F4" s="6">
         <v>0</v>
       </c>
       <c r="G4" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H4" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I4" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J4" s="6">
         <v>0</v>
@@ -2229,97 +2172,34 @@
         <v>0</v>
       </c>
       <c r="L4" s="6">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2328,10 +2208,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20090B-02A9-43B7-8D03-9C18D42920EB}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2356,13 +2236,13 @@
         <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>15</v>
@@ -2377,21 +2257,21 @@
         <v>16</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
@@ -2433,7 +2313,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B3" s="6">
         <v>0</v>
@@ -2448,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
@@ -2474,118 +2354,19 @@
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>3</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
       <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>1</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2653,10 +2434,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,19 +2458,19 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>19</v>
@@ -2698,15 +2479,15 @@
         <v>18</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>7</v>
@@ -2732,13 +2513,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" s="8">
         <v>1</v>
@@ -2761,19 +2542,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D4" s="8">
         <v>1</v>
       </c>
       <c r="E4" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -2790,22 +2571,22 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="E5" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
@@ -2814,122 +2595,6 @@
         <v>1</v>
       </c>
       <c r="I5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2954,7 +2619,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -2970,9 +2635,9 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -3118,10 +2783,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3146,7 +2811,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1"/>
     </row>
@@ -3165,9 +2830,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -3320,7 +2985,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3340,9 +3005,9 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="7" t="str">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
-        <v>44671.08333321759</v>
+        <v/>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>

</xml_diff>